<commit_message>
add Type Delivery table
</commit_message>
<xml_diff>
--- a/files/management/commands/price.xlsx
+++ b/files/management/commands/price.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="uf-print" sheetId="4" r:id="rId1"/>
-    <sheet name="type_print" sheetId="5" r:id="rId2"/>
-    <sheet name="status_product" sheetId="6" r:id="rId3"/>
-    <sheet name="shirka" sheetId="1" r:id="rId4"/>
-    <sheet name="interierka" sheetId="3" r:id="rId5"/>
-    <sheet name="finishka" sheetId="2" r:id="rId6"/>
+    <sheet name="delivery" sheetId="8" r:id="rId1"/>
+    <sheet name="status_order" sheetId="7" r:id="rId2"/>
+    <sheet name="uf-print" sheetId="4" r:id="rId3"/>
+    <sheet name="type_print" sheetId="5" r:id="rId4"/>
+    <sheet name="status_product" sheetId="6" r:id="rId5"/>
+    <sheet name="shirka" sheetId="1" r:id="rId6"/>
+    <sheet name="interierka" sheetId="3" r:id="rId7"/>
+    <sheet name="finishka" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Название</t>
   </si>
@@ -182,6 +184,24 @@
   </si>
   <si>
     <t>Статус продукта</t>
+  </si>
+  <si>
+    <t>Готовится</t>
+  </si>
+  <si>
+    <t>Передан в доставку</t>
+  </si>
+  <si>
+    <t>Завешен</t>
+  </si>
+  <si>
+    <t>Статус Заказа</t>
+  </si>
+  <si>
+    <t>Типы доставки</t>
+  </si>
+  <si>
+    <t>Самовывоз</t>
   </si>
 </sst>
 </file>
@@ -553,6 +573,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -695,7 +855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -762,11 +922,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -809,7 +969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H68"/>
   <sheetViews>
@@ -1637,7 +1797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -2023,7 +2183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>

</xml_diff>

<commit_message>
del add test.py data_test.py
</commit_message>
<xml_diff>
--- a/files/management/commands/price.xlsx
+++ b/files/management/commands/price.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="delivery" sheetId="8" r:id="rId1"/>
@@ -575,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1801,7 +1801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add load Blank material price from excel
</commit_message>
<xml_diff>
--- a/files/management/commands/price.xlsx
+++ b/files/management/commands/price.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="delivery" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="type_print" sheetId="4" r:id="rId4"/>
     <sheet name="status_product" sheetId="5" r:id="rId5"/>
     <sheet name="shirka" sheetId="6" r:id="rId6"/>
-    <sheet name="interierka" sheetId="7" r:id="rId7"/>
-    <sheet name="finishka" sheetId="8" r:id="rId8"/>
+    <sheet name="blank_material" sheetId="9" r:id="rId7"/>
+    <sheet name="interierka" sheetId="7" r:id="rId8"/>
+    <sheet name="finishka" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>№</t>
   </si>
@@ -940,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1763,6 +1764,198 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7">
+        <v>100</v>
+      </c>
+      <c r="D2" s="7">
+        <f>C2*2</f>
+        <v>200</v>
+      </c>
+      <c r="E2" s="7">
+        <f>D2*1.3</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="7">
+        <v>125</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D9" si="0">C3*2</f>
+        <v>250</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E9" si="1">D3*1.3</f>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7">
+        <v>140</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="1"/>
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="7">
+        <v>165</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="1"/>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="7">
+        <v>230</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="1"/>
+        <v>598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="7">
+        <v>110</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="1"/>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="7">
+        <v>250</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="7">
+        <v>120</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="1"/>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -2149,12 +2342,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add logo + edit price.xlsx
</commit_message>
<xml_diff>
--- a/files/management/commands/price.xlsx
+++ b/files/management/commands/price.xlsx
@@ -1,38 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileSharing readOnlyRecommended="0" userName="sasha"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasha\PycharmProjects\tiff_django\files\management\commands\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
+    <workbookView activeTab="8" xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="delivery" sheetId="1" r:id="rId1"/>
-    <sheet name="status_order" sheetId="2" r:id="rId2"/>
-    <sheet name="uf-print" sheetId="3" r:id="rId3"/>
-    <sheet name="type_print" sheetId="4" r:id="rId4"/>
-    <sheet name="status_product" sheetId="5" r:id="rId5"/>
-    <sheet name="shirka" sheetId="6" r:id="rId6"/>
-    <sheet name="blank_material" sheetId="9" r:id="rId7"/>
-    <sheet name="interierka" sheetId="7" r:id="rId8"/>
-    <sheet name="finishka" sheetId="8" r:id="rId9"/>
+    <sheet name="delivery" sheetId="1" r:id="rId4"/>
+    <sheet name="status_order" sheetId="2" r:id="rId5"/>
+    <sheet name="uf-print" sheetId="3" r:id="rId6"/>
+    <sheet name="type_print" sheetId="4" r:id="rId7"/>
+    <sheet name="status_product" sheetId="5" r:id="rId8"/>
+    <sheet name="shirka" sheetId="6" r:id="rId9"/>
+    <sheet name="blank_material" sheetId="7" r:id="rId10"/>
+    <sheet name="interierka" sheetId="8" r:id="rId11"/>
+    <sheet name="finishka" sheetId="9" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+    <ext uri="smNativeData">
+      <pm:revision xmlns:pm="smNativeData" day="1722022763" val="1216" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1722022763" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1722022763" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1722022763"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>№</t>
   </si>
@@ -184,7 +183,7 @@
     <t xml:space="preserve">Холст </t>
   </si>
   <si>
-    <t>Без обработки (оставить белые поля)</t>
+    <t>оставить белые поля по 5 см</t>
   </si>
   <si>
     <t>Резка в размер (обрезка полей по краю изображения)</t>
@@ -203,62 +202,89 @@
   </si>
   <si>
     <t>Люверсы проварка со шнуром</t>
+  </si>
+  <si>
+    <t>Без полей</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="#,##0\ &quot;₽&quot;;\-#,##0\ &quot;₽&quot;"/>
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;₽&quot;;[Red]\-#,##0\ &quot;₽&quot;"/>
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;₽&quot;;\-#,##0.00\ &quot;₽&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;₽&quot;;[Red]\-#,##0.00\ &quot;₽&quot;"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4">
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1722022763" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="Basic Sans"/>
+      <family val="1"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color theme="1"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1722022763" ulstyle="none" kern="1">
+            <pm:latin face="Basic Sans" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="204"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1722022763" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="240" lang="default" weight="bold"/>
+            <pm:cs face="Basic Roman" sz="240" lang="default" weight="bold"/>
+            <pm:ea face="Basic Roman" sz="240" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
+      <color rgb="FF000000"/>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1722022763" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="240" lang="default"/>
+            <pm:cs face="Basic Roman" sz="240" lang="default"/>
+            <pm:ea face="Basic Roman" sz="240" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,291 +293,539 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59987182226020086"/>
-        <bgColor rgb="FF99CC00"/>
+        <fgColor rgb="FF88FD77"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="0088FD77" bgLvl="0" bgClr="0099CC00"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBF819E"/>
-        <bgColor rgb="FF808080"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="00BF819E" bgLvl="0" bgClr="00808080"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
-        <bgColor rgb="FF008000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="0000A933" bgLvl="0" bgClr="00008000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFB66C"/>
-        <bgColor rgb="FFFF99CC"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="00FFB66C" bgLvl="0" bgClr="00FF99CC"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00993300"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
+        </ext>
+      </extLst>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF89FD78"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFB66C"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FFBF819E"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF00A933"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="smNativeData">
+      <pm:charStyles xmlns:pm="smNativeData" id="1722022763" count="1">
+        <pm:charStyle name="Обычный" fontId="0" Id="1"/>
+      </pm:charStyles>
+      <pm:colors xmlns:pm="smNativeData" id="1722022763" count="9">
+        <pm:color name="Цвет 24" rgb="88FD77"/>
+        <pm:color name="Цвет 25" rgb="99CC00"/>
+        <pm:color name="Цвет 26" rgb="BF819E"/>
+        <pm:color name="Цвет 27" rgb="808080"/>
+        <pm:color name="Цвет 28" rgb="00A933"/>
+        <pm:color name="Цвет 29" rgb="008000"/>
+        <pm:color name="Цвет 30" rgb="FFB66C"/>
+        <pm:color name="Цвет 31" rgb="FF99CC"/>
+        <pm:color name="Цвет 32" rgb="993300"/>
+      </pm:colors>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="LibreOffice">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="EEECE1"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="1F497D"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:ea typeface="Basic Roman"/>
+        <a:cs typeface="Basic Roman"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter/>
         </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter/>
         </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr>
+        <a:prstTxWarp prst="textNoShape">
+          <a:avLst/>
+        </a:prstTxWarp>
+        <a:noAutofit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr>
+          <a:defRPr/>
+        </a:defPPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.000000" customWidth="1"/>
+    <col min="2" max="2" width="18.567568" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,65 +833,88 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:2">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:2">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:2">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:2">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:2">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.000000" customWidth="1"/>
+    <col min="2" max="2" width="18.567568" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -625,48 +922,48 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:2">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:2">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:2">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:2">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:2">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -674,29 +971,52 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.45"/>
   <cols>
-    <col min="2" max="2" width="58.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="2" max="2" width="58.423423" customWidth="1"/>
+    <col min="3" max="3" width="16.567568" customWidth="1"/>
+    <col min="4" max="4" width="21.855856" customWidth="1"/>
+    <col min="5" max="5" width="28.567568" customWidth="1"/>
+    <col min="6" max="6" width="31.000000" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -714,127 +1034,152 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="7" t="n">
         <v>1400</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="7" t="n">
         <v>3600</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="7" t="n">
         <v>3600</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="7" t="n">
         <v>2020</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="7" t="n">
         <v>4200</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="7" t="n">
         <v>3600</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="7" t="n">
         <v>1700</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="7" t="n">
         <v>3600</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="7" t="n">
         <v>3600</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="7" t="n">
         <v>425</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="7" t="n">
         <v>850</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="7" t="n">
         <v>1600</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="6" spans="1:6">
+      <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="7" t="n">
         <v>425</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="7" t="n">
         <v>850</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="7" t="n">
         <v>1600</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="6:6">
       <c r="F7" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.45"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.423423" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,8 +1187,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:5">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -853,8 +1198,8 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:5">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -864,8 +1209,8 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:5">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -875,8 +1220,8 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:2">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -884,22 +1229,45 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -907,24 +1275,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:2">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:2">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -932,30 +1300,53 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="A10" sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.567568" defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="56.5703125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.855856" customWidth="1" style="10"/>
+    <col min="2" max="2" width="56.567568" customWidth="1" style="10"/>
+    <col min="3" max="3" width="16.567568" customWidth="1" style="10"/>
+    <col min="4" max="4" width="21.144144" customWidth="1" style="10"/>
+    <col min="5" max="5" width="27.423423" customWidth="1" style="10"/>
+    <col min="6" max="6" width="28.423423" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="5"/>
       <c r="B1" s="11" t="s">
         <v>10</v>
@@ -975,205 +1366,205 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="2" spans="1:8">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="7" t="n">
         <v>185</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="7" t="n">
         <v>350</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="7" t="n">
         <v>72</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+    <row r="3" spans="1:8">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="7" t="n">
         <v>255</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="7" t="n">
         <v>440</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="7" t="n">
         <v>500</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="7" t="n">
         <v>72</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+    <row r="4" spans="1:8">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="7" t="n">
         <v>320</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="7" t="n">
         <v>620</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="7" t="n">
         <v>700</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="7" t="n">
         <v>72</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="7" t="n">
         <v>450</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="7" t="n">
         <v>72</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="6" spans="1:8">
+      <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="7" t="n">
         <v>165</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="7" t="n">
         <v>280</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="7" t="n">
         <v>340</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="7" t="n">
         <v>72</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+    <row r="7" spans="1:8">
+      <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="7" t="n">
         <v>230</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="7" t="n">
         <v>395</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="7" t="n">
         <v>420</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="7" t="n">
         <v>72</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+    <row r="8" spans="1:8">
+      <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="7" t="n">
         <v>110</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="7" t="n">
         <v>220</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="7" t="n">
         <v>330</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="7" t="n">
         <v>72</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+    <row r="9" spans="1:8">
+      <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="7" t="n">
         <v>250</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="7" t="n">
         <v>425</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="7" t="n">
         <v>500</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="7" t="n">
         <v>72</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+    <row r="10" spans="1:8">
+      <c r="A10" s="5" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="7" t="n">
         <v>255</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="7" t="n">
         <v>300</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="7" t="n">
         <v>72</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="7"/>
@@ -1183,7 +1574,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="7"/>
@@ -1193,7 +1584,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="7"/>
@@ -1203,7 +1594,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="7"/>
@@ -1213,7 +1604,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="7"/>
@@ -1223,7 +1614,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="7"/>
@@ -1233,7 +1624,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="7"/>
@@ -1243,7 +1634,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="7"/>
@@ -1253,7 +1644,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="7"/>
@@ -1263,7 +1654,7 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="7"/>
@@ -1273,7 +1664,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="7"/>
@@ -1283,7 +1674,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="7"/>
@@ -1293,7 +1684,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="7"/>
@@ -1303,7 +1694,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="7"/>
@@ -1313,7 +1704,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="7"/>
@@ -1323,7 +1714,7 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="7"/>
@@ -1333,7 +1724,7 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1343,7 +1734,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1353,7 +1744,7 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1363,7 +1754,7 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1373,7 +1764,7 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1383,7 +1774,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1393,7 +1784,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1403,7 +1794,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1413,7 +1804,7 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1423,7 +1814,7 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1433,7 +1824,7 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1443,7 +1834,7 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1453,7 +1844,7 @@
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1463,7 +1854,7 @@
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1473,7 +1864,7 @@
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1483,7 +1874,7 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1493,7 +1884,7 @@
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
     </row>
-    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1503,7 +1894,7 @@
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1513,7 +1904,7 @@
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1523,7 +1914,7 @@
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1533,7 +1924,7 @@
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1543,7 +1934,7 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -1553,7 +1944,7 @@
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1563,7 +1954,7 @@
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -1573,7 +1964,7 @@
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -1583,7 +1974,7 @@
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -1593,7 +1984,7 @@
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -1603,7 +1994,7 @@
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -1613,7 +2004,7 @@
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -1623,7 +2014,7 @@
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -1633,7 +2024,7 @@
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -1643,7 +2034,7 @@
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -1653,7 +2044,7 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -1663,7 +2054,7 @@
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
     </row>
-    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -1673,7 +2064,7 @@
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -1683,7 +2074,7 @@
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -1693,7 +2084,7 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -1703,7 +2094,7 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -1713,7 +2104,7 @@
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -1723,7 +2114,7 @@
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
     </row>
-    <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -1733,7 +2124,7 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -1743,7 +2134,7 @@
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
     </row>
-    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -1754,33 +2145,54 @@
       <c r="H68" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.787500" right="0.787500" top="1.052778" bottom="1.052778" header="0.787500" footer="0.787500"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1" useFirstPageNumber="1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman"&amp;12Page &amp;P</oddFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
   </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.567568" customWidth="1"/>
+    <col min="2" max="2" width="58.423423" customWidth="1"/>
+    <col min="3" max="3" width="16.567568" customWidth="1"/>
+    <col min="4" max="4" width="21.855856" customWidth="1"/>
+    <col min="5" max="5" width="28.567568" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="5"/>
       <c r="B1" s="11" t="s">
         <v>10</v>
@@ -1795,168 +2207,192 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="2" spans="1:5">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="7" t="n">
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+    <row r="3" spans="1:5">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="7" t="n">
         <v>125</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="7" t="n">
         <v>250</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="7" t="n">
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+    <row r="4" spans="1:5">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="7" t="n">
         <v>140</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="7" t="n">
         <v>280</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="7" t="n">
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+    <row r="5" spans="1:5">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="7" t="n">
         <v>165</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="7" t="n">
         <v>330</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="7" t="n">
         <v>430</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="7" t="n">
         <v>230</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="7" t="n">
         <v>460</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="7" t="n">
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+    <row r="7" spans="1:5">
+      <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="7" t="n">
         <v>110</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="7" t="n">
         <v>220</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="7" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+    <row r="8" spans="1:5">
+      <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="7" t="n">
         <v>250</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="7" t="n">
         <v>500</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="7" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5">
+      <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="7" t="n">
         <v>240</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="7" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.45"/>
   <cols>
-    <col min="2" max="2" width="58.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="2" max="2" width="58.423423" customWidth="1"/>
+    <col min="3" max="3" width="16.567568" customWidth="1"/>
+    <col min="4" max="4" width="21.855856" customWidth="1"/>
+    <col min="5" max="5" width="28.567568" customWidth="1"/>
+    <col min="6" max="6" width="31.000000" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1974,376 +2410,399 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="7" t="n">
         <v>350</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="7" t="n">
         <v>700</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="7" t="n">
         <v>750</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="7" t="n">
         <v>800</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="7" t="n">
         <v>450</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="7" t="n">
         <v>1100</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="7" t="n">
         <v>1100</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="7" t="n">
         <v>520</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="7" t="n">
         <v>1100</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="7" t="n">
         <v>1600</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="6" spans="1:6">
+      <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="7" t="n">
         <v>380</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="7" t="n">
         <v>760</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="7" t="n">
         <v>760</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="7" t="n">
         <v>320</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="7" t="n">
         <v>520</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="7" t="n">
         <v>650</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="7" t="n">
         <v>320</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="7" t="n">
         <v>520</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="7" t="n">
         <v>650</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+    <row r="9" spans="1:6">
+      <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="7" t="n">
         <v>580</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="7" t="n">
         <v>850</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="7" t="n">
         <v>1100</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+    <row r="10" spans="1:6">
+      <c r="A10" s="5" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="7" t="n">
         <v>270</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="7" t="n">
         <v>410</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="7" t="n">
         <v>410</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+    <row r="11" spans="1:6">
+      <c r="A11" s="5" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="7" t="n">
         <v>450</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+    <row r="12" spans="1:6">
+      <c r="A12" s="5" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="7" t="n">
         <v>450</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+    <row r="13" spans="1:6">
+      <c r="A13" s="5" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="7" t="n">
         <v>450</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+    <row r="14" spans="1:6">
+      <c r="A14" s="5" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="7" t="n">
         <v>450</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+    <row r="15" spans="1:6">
+      <c r="A15" s="5" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="7" t="n">
         <v>500</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="7" t="n">
         <v>1000</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="7" t="n">
         <v>1000</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+    <row r="16" spans="1:6">
+      <c r="A16" s="5" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="7" t="n">
         <v>500</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="7" t="n">
         <v>1000</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="7" t="n">
         <v>1000</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+    <row r="17" spans="1:6">
+      <c r="A17" s="5" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="7" t="n">
         <v>250</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="7" t="n">
         <v>1400</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+    <row r="18" spans="1:6">
+      <c r="A18" s="5" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="7" t="n">
         <v>750</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="7" t="n">
         <v>1400</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="7" t="n">
         <v>1400</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="7" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:6">
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:6">
       <c r="F20" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.567568" defaultRowHeight="13.45"/>
   <cols>
-    <col min="2" max="2" width="57.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="57.423423" customWidth="1" style="10"/>
+    <col min="3" max="3" width="16.288288" customWidth="1" style="10"/>
+    <col min="4" max="4" width="21.144144" customWidth="1" style="10"/>
+    <col min="5" max="5" width="27.423423" customWidth="1" style="10"/>
+    <col min="6" max="6" width="28.423423" customWidth="1" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="5"/>
       <c r="B1" s="11" t="s">
         <v>10</v>
@@ -2364,20 +2823,20 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="2" spans="1:12">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="5"/>
@@ -2387,20 +2846,20 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+    <row r="3" spans="1:12">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="7" t="n">
         <v>45</v>
       </c>
       <c r="G3" s="5"/>
@@ -2410,20 +2869,20 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+    <row r="4" spans="1:12">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="7" t="n">
         <v>150</v>
       </c>
       <c r="G4" s="5"/>
@@ -2433,20 +2892,20 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+    <row r="5" spans="1:12">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="7" t="n">
         <v>80</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="7" t="n">
         <v>150</v>
       </c>
       <c r="G5" s="5"/>
@@ -2456,20 +2915,20 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="6" spans="1:12">
+      <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="7" t="n">
         <v>180</v>
       </c>
       <c r="G6" s="5"/>
@@ -2479,20 +2938,20 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+    <row r="7" spans="1:12">
+      <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="7" t="n">
         <v>180</v>
       </c>
       <c r="G7" s="5"/>
@@ -2502,20 +2961,20 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+    <row r="8" spans="1:12">
+      <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="7" t="n">
         <v>240</v>
       </c>
       <c r="F8" s="5"/>
@@ -2526,11 +2985,22 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+    <row r="9" spans="1:12">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -2539,7 +3009,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2553,7 +3023,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2567,7 +3037,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2581,7 +3051,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2595,7 +3065,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2609,7 +3079,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2623,7 +3093,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2637,7 +3107,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2651,7 +3121,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2665,7 +3135,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2679,7 +3149,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2693,7 +3163,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2707,7 +3177,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2721,7 +3191,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2735,7 +3205,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2749,7 +3219,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2763,7 +3233,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2777,7 +3247,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2791,7 +3261,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2805,7 +3275,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2819,7 +3289,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2833,7 +3303,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2847,7 +3317,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2861,7 +3331,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2875,7 +3345,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2889,7 +3359,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2903,7 +3373,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2917,7 +3387,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2931,7 +3401,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2945,7 +3415,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2959,7 +3429,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2973,7 +3443,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2987,7 +3457,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -3001,7 +3471,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -3016,11 +3486,32 @@
       <c r="L43" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.787500" right="0.787500" top="1.052778" bottom="1.052778" header="0.787500" footer="0.787500"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman"&amp;12Page &amp;P</oddFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
   </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create phone in User del fields in profile
</commit_message>
<xml_diff>
--- a/files/management/commands/price.xlsx
+++ b/files/management/commands/price.xlsx
@@ -1,30 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="sasha"/>
-  <workbookPr/>
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="8" xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="delivery" sheetId="1" r:id="rId4"/>
-    <sheet name="status_order" sheetId="2" r:id="rId5"/>
-    <sheet name="uf-print" sheetId="3" r:id="rId6"/>
-    <sheet name="type_print" sheetId="4" r:id="rId7"/>
-    <sheet name="status_product" sheetId="5" r:id="rId8"/>
-    <sheet name="shirka" sheetId="6" r:id="rId9"/>
-    <sheet name="blank_material" sheetId="7" r:id="rId10"/>
-    <sheet name="interierka" sheetId="8" r:id="rId11"/>
-    <sheet name="finishka" sheetId="9" r:id="rId12"/>
+    <sheet name="delivery" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="status_order" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="uf-print" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="type_print" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="status_product" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="shirka" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="blank_material" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="interierka" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="finishka" sheetId="9" state="visible" r:id="rId11"/>
   </sheets>
-  <calcPr iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1722022763" val="1216" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1722022763" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1722022763" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1722022763"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -33,258 +30,227 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
-    <t>№</t>
-  </si>
-  <si>
-    <t>Типы доставки</t>
-  </si>
-  <si>
-    <t>Самовывоз</t>
-  </si>
-  <si>
-    <t>Статус Заказа</t>
-  </si>
-  <si>
-    <t>Готовится</t>
-  </si>
-  <si>
-    <t>Оформлен</t>
-  </si>
-  <si>
-    <t>В работе</t>
-  </si>
-  <si>
-    <t>Передан в доставку</t>
-  </si>
-  <si>
-    <t>Готов</t>
-  </si>
-  <si>
-    <t>Завешен</t>
-  </si>
-  <si>
-    <t>Название</t>
-  </si>
-  <si>
-    <t>Цена закупки</t>
-  </si>
-  <si>
-    <t>Цена продажи РА</t>
-  </si>
-  <si>
-    <t>Цена продажи Розница</t>
-  </si>
-  <si>
-    <t>Разрешение печати в DPI</t>
-  </si>
-  <si>
-    <t>Печать на ПВХ 3 мм</t>
-  </si>
-  <si>
-    <t>Печать на ПВХ 5 мм</t>
-  </si>
-  <si>
-    <t>Печать на оцинковке</t>
-  </si>
-  <si>
-    <t>Печать на на пленке матовая 100 мик</t>
-  </si>
-  <si>
-    <t>Печать на на пленке глянцевая 100 мик</t>
-  </si>
-  <si>
-    <t>Типы Печати</t>
-  </si>
-  <si>
-    <t>Широкоформатная печать</t>
-  </si>
-  <si>
-    <t>Интерьерная печать</t>
-  </si>
-  <si>
-    <t>UV-печать</t>
-  </si>
-  <si>
-    <t>Чистый материал</t>
-  </si>
-  <si>
-    <t>Статус продукта</t>
-  </si>
-  <si>
-    <t>Баннер 440 грамм ламинированный</t>
-  </si>
-  <si>
-    <t>Баннер 510 грамм литой</t>
-  </si>
-  <si>
-    <t>Баннер 510 грамм литой (Черный оборот)</t>
-  </si>
-  <si>
-    <t>Баннер 510 грамм литой (Черный оборот Без печати)</t>
-  </si>
-  <si>
-    <t>Баннер 340 грамм ламинированный</t>
-  </si>
-  <si>
-    <t>Пленка самоклеющаяся</t>
-  </si>
-  <si>
-    <t>Блюбек</t>
-  </si>
-  <si>
-    <t>Баннерная сетка 370 грамм</t>
+    <t xml:space="preserve">№</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Типы доставки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Самовывоз</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Статус Заказа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Готовится</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Оформлен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В работе</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Передан в доставку</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Готов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Завешен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Название</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена закупки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена продажи РА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена продажи Розница</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разрешение печати в DPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Печать на ПВХ 3 мм</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Печать на ПВХ 5 мм</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Печать на оцинковке</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Печать на на пленке матовая 100 мик</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Печать на на пленке глянцевая 100 мик</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Типы Печати</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Широкоформатная печать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Интерьерная печать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UV-печать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чистый материал</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Статус продукта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Баннер 440 грамм ламинированный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Баннер 510 грамм литой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Баннер 510 грамм литой (Черный оборот)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Баннер 510 грамм литой (Черный оборот Без печати)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Баннер 340 грамм ламинированный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пленка самоклеющаяся</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Блюбек</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Баннерная сетка 370 грамм</t>
   </si>
   <si>
     <t xml:space="preserve">Бумага 150 грамм СytiLight </t>
   </si>
   <si>
-    <t>Баннер 440 гр ламинированный</t>
-  </si>
-  <si>
-    <t>Беклит матовый 260 гр</t>
-  </si>
-  <si>
-    <t>Печать на пленке с контурной резкой</t>
-  </si>
-  <si>
-    <t>Пленка перфорированная (черный оборот)</t>
-  </si>
-  <si>
-    <t>Пленка Китай 100 мкр Матовая</t>
-  </si>
-  <si>
-    <t>Пленка Китай 100 мкр Глянец</t>
+    <t xml:space="preserve">Баннер 440 гр ламинированный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Беклит матовый 260 гр</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Печать на пленке с контурной резкой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пленка перфорированная (черный оборот)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пленка Китай 100 мкр Матовая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пленка Китай 100 мкр Глянец</t>
   </si>
   <si>
     <t xml:space="preserve">Пленка Китай 100 мик Глянец + ламинация </t>
   </si>
   <si>
-    <t>Пленка Oraget матовая</t>
-  </si>
-  <si>
-    <t>Пленка Oraget глянцевая</t>
-  </si>
-  <si>
-    <t>Пленка Oraget прозрачная матовая</t>
-  </si>
-  <si>
-    <t>Пленка Oraget прозрачная глянцевая</t>
-  </si>
-  <si>
-    <t>Фотобумага Глянец 200 гр</t>
-  </si>
-  <si>
-    <t>Фотобумага Матовая 200 гр</t>
-  </si>
-  <si>
-    <t>Фотообои</t>
+    <t xml:space="preserve">Пленка Oraget матовая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пленка Oraget глянцевая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пленка Oraget прозрачная матовая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пленка Oraget прозрачная глянцевая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фотобумага Глянец 200 гр</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фотобумага Матовая 200 гр</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фотообои</t>
   </si>
   <si>
     <t xml:space="preserve">Холст </t>
   </si>
   <si>
-    <t>оставить белые поля по 5 см</t>
-  </si>
-  <si>
-    <t>Резка в размер (обрезка полей по краю изображения)</t>
-  </si>
-  <si>
-    <t>Люверсы по углам</t>
-  </si>
-  <si>
-    <t>Люверсы через 30 см с проваркой</t>
-  </si>
-  <si>
-    <t>Проварка кармана сверху</t>
-  </si>
-  <si>
-    <t>Проварка кармана снизу</t>
-  </si>
-  <si>
-    <t>Люверсы проварка со шнуром</t>
-  </si>
-  <si>
-    <t>Без полей</t>
+    <t xml:space="preserve">оставить белые поля по 5 см</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Резка в размер (обрезка полей по краю изображения)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Люверсы по углам</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Люверсы через 30 см с проваркой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проварка кармана сверху</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проварка кармана снизу</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Люверсы проварка со шнуром</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Без полей</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="#,##0\ &quot;₽&quot;;\-#,##0\ &quot;₽&quot;"/>
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;₽&quot;;[Red]\-#,##0\ &quot;₽&quot;"/>
-    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;₽&quot;;\-#,##0.00\ &quot;₽&quot;"/>
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;₽&quot;;[Red]\-#,##0.00\ &quot;₽&quot;"/>
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1722022763" ulstyle="none" kern="1">
-            <pm:latin face="Arial" sz="200" lang="default"/>
-            <pm:cs face="Basic Roman" sz="200" lang="default"/>
-            <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Basic Sans"/>
-      <family val="1"/>
-      <color rgb="FF000000"/>
       <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1722022763" ulstyle="none" kern="1">
-            <pm:latin face="Basic Sans" sz="200" lang="default"/>
-            <pm:cs face="Basic Roman" sz="200" lang="default"/>
-            <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1722022763" ulstyle="none" kern="1">
-            <pm:latin face="Arial" sz="240" lang="default" weight="bold"/>
-            <pm:cs face="Basic Roman" sz="240" lang="default" weight="bold"/>
-            <pm:ea face="Basic Roman" sz="240" lang="default" weight="bold"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1722022763" ulstyle="none" kern="1">
-            <pm:latin face="Arial" sz="240" lang="default"/>
-            <pm:cs face="Basic Roman" sz="240" lang="default"/>
-            <pm:ea face="Basic Roman" sz="240" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,305 +260,229 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF88FD77"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="0088FD77" bgLvl="0" bgClr="0099CC00"/>
-          </ext>
-        </extLst>
+        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBF819E"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="00BF819E" bgLvl="0" bgClr="00808080"/>
-          </ext>
-        </extLst>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="0000A933" bgLvl="0" bgClr="00008000"/>
-          </ext>
-        </extLst>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFB66C"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="00FFB66C" bgLvl="0" bgClr="00FF99CC"/>
-          </ext>
-        </extLst>
+        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00993300"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1722022763" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1722022763"/>
-        </ext>
-      </extLst>
+  <borders count="1">
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+  <cellXfs count="13">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0"/>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1722022763" count="1">
-        <pm:charStyle name="Обычный" fontId="0" Id="1"/>
-      </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1722022763" count="9">
-        <pm:color name="Цвет 24" rgb="88FD77"/>
-        <pm:color name="Цвет 25" rgb="99CC00"/>
-        <pm:color name="Цвет 26" rgb="BF819E"/>
-        <pm:color name="Цвет 27" rgb="808080"/>
-        <pm:color name="Цвет 28" rgb="00A933"/>
-        <pm:color name="Цвет 29" rgb="008000"/>
-        <pm:color name="Цвет 30" rgb="FFB66C"/>
-        <pm:color name="Цвет 31" rgb="FF99CC"/>
-        <pm:color name="Цвет 32" rgb="993300"/>
-      </pm:colors>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF88FD77"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFB66C"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FFBF819E"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="eeece1"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="1f497d"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4f81bd"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="c0504d"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="9bbb59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="8064a2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4bacc6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="f79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0000ff"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -600,232 +490,156 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Basic Roman"/>
-        <a:cs typeface="Basic Roman"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Basic Roman" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Basic Roman" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
-                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
-                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
-                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr>
-        <a:prstTxWarp prst="textNoShape">
-          <a:avLst/>
-        </a:prstTxWarp>
-        <a:noAutofit/>
-      </a:bodyPr>
-      <a:lstStyle>
-        <a:defPPr>
-          <a:defRPr/>
-        </a:defPPr>
-      </a:lstStyle>
-      <a:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3.000000" customWidth="1"/>
-    <col min="2" max="2" width="18.567568" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -833,88 +647,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="n">
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="n">
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="n">
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="n">
+    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="n">
+    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="n">
+    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3.000000" customWidth="1"/>
-    <col min="2" max="2" width="18.567568" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,48 +721,48 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="n">
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="n">
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="n">
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="n">
+    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="n">
+    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="n">
+    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -971,52 +770,37 @@
       </c>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="58.423423" customWidth="1"/>
-    <col min="3" max="3" width="16.567568" customWidth="1"/>
-    <col min="4" max="4" width="21.855856" customWidth="1"/>
-    <col min="5" max="5" width="28.567568" customWidth="1"/>
-    <col min="6" max="6" width="31.000000" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1034,152 +818,137 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="6" t="n">
         <v>1400</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>3600</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="6" t="n">
         <v>3600</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="6" t="n">
         <v>2020</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="6" t="n">
         <v>4200</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="6" t="n">
         <v>3600</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="6" t="n">
         <v>1700</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>3600</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="6" t="n">
         <v>3600</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>425</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>850</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>1600</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="6" t="n">
         <v>425</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>850</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="6" t="n">
         <v>1600</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="6:6">
-      <c r="F7" s="8"/>
+    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="7"/>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="23.423423" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1187,41 +956,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="n">
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="n">
+    </row>
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="n">
+    </row>
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="n">
+    </row>
+    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1229,45 +989,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1275,24 +1020,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="n">
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="n">
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="n">
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1300,64 +1045,49 @@
       </c>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.567568" defaultRowHeight="13.45"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2.855856" customWidth="1" style="10"/>
-    <col min="2" max="2" width="56.567568" customWidth="1" style="10"/>
-    <col min="3" max="3" width="16.567568" customWidth="1" style="10"/>
-    <col min="4" max="4" width="21.144144" customWidth="1" style="10"/>
-    <col min="5" max="5" width="27.423423" customWidth="1" style="10"/>
-    <col min="6" max="6" width="28.423423" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -1366,365 +1096,365 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="6" t="n">
         <v>185</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>350</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="6" t="n">
         <v>400</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="6" t="n">
         <v>72</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="6" t="n">
         <v>255</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="6" t="n">
         <v>440</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="6" t="n">
         <v>500</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="6" t="n">
         <v>72</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="6" t="n">
         <v>320</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>620</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="6" t="n">
         <v>700</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="6" t="n">
         <v>72</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>200</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>400</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>72</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="6" t="n">
         <v>165</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>280</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="6" t="n">
         <v>340</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="6" t="n">
         <v>72</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>230</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="6" t="n">
         <v>395</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="6" t="n">
         <v>420</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="6" t="n">
         <v>72</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="6" t="n">
         <v>110</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>220</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="6" t="n">
         <v>330</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="6" t="n">
         <v>72</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="6" t="n">
         <v>250</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="6" t="n">
         <v>425</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="6" t="n">
         <v>500</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="6" t="n">
         <v>72</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="6" t="n">
         <v>255</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="6" t="n">
         <v>300</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="6" t="n">
         <v>72</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1734,7 +1464,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1744,7 +1474,7 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1754,7 +1484,7 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1764,7 +1494,7 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1774,7 +1504,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1784,7 +1514,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1794,7 +1524,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1804,7 +1534,7 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1814,7 +1544,7 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1824,7 +1554,7 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1834,7 +1564,7 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1844,7 +1574,7 @@
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1854,7 +1584,7 @@
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1864,7 +1594,7 @@
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1874,7 +1604,7 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1884,7 +1614,7 @@
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1894,7 +1624,7 @@
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1904,7 +1634,7 @@
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1914,7 +1644,7 @@
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1924,7 +1654,7 @@
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1934,7 +1664,7 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -1944,7 +1674,7 @@
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1954,7 +1684,7 @@
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -1964,7 +1694,7 @@
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -1974,7 +1704,7 @@
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -1984,7 +1714,7 @@
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -1994,7 +1724,7 @@
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2004,7 +1734,7 @@
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2014,7 +1744,7 @@
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -2024,7 +1754,7 @@
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -2034,7 +1764,7 @@
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2044,7 +1774,7 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2054,7 +1784,7 @@
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2064,7 +1794,7 @@
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -2074,7 +1804,7 @@
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -2084,7 +1814,7 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2094,7 +1824,7 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -2104,7 +1834,7 @@
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -2114,7 +1844,7 @@
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -2124,7 +1854,7 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -2134,7 +1864,7 @@
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -2145,254 +1875,222 @@
       <c r="H68" s="5"/>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.787500" right="0.787500" top="1.052778" bottom="1.052778" header="0.787500" footer="0.787500"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1" useFirstPageNumber="1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman"&amp;12Page &amp;P</oddFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2.567568" customWidth="1"/>
-    <col min="2" max="2" width="58.423423" customWidth="1"/>
-    <col min="3" max="3" width="16.567568" customWidth="1"/>
-    <col min="4" max="4" width="21.855856" customWidth="1"/>
-    <col min="5" max="5" width="28.567568" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="6" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>200</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="6" t="n">
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="6" t="n">
         <v>125</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="6" t="n">
         <v>250</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="6" t="n">
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="6" t="n">
         <v>140</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>280</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="6" t="n">
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>165</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>330</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>430</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="6" t="n">
         <v>230</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>460</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="6" t="n">
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>110</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="6" t="n">
         <v>220</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="6" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="6" t="n">
         <v>250</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>500</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="6" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="6" t="n">
         <v>240</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="6" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="58.423423" customWidth="1"/>
-    <col min="3" max="3" width="16.567568" customWidth="1"/>
-    <col min="4" max="4" width="21.855856" customWidth="1"/>
-    <col min="5" max="5" width="28.567568" customWidth="1"/>
-    <col min="6" max="6" width="31.000000" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -2410,410 +2108,395 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="6" t="n">
         <v>350</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>700</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="6" t="n">
         <v>750</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="6" t="n">
         <v>400</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="6" t="n">
         <v>800</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>1100</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="6" t="n">
         <v>1100</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>520</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>1100</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>1600</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="6" t="n">
         <v>380</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>760</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="6" t="n">
         <v>760</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>320</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="6" t="n">
         <v>520</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="6" t="n">
         <v>650</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="6" t="n">
         <v>320</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>520</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="6" t="n">
         <v>650</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="6" t="n">
         <v>580</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="6" t="n">
         <v>850</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="6" t="n">
         <v>1100</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="6" t="n">
         <v>270</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="6" t="n">
         <v>410</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="6" t="n">
         <v>410</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="F11" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="E12" s="7" t="n">
+      <c r="E12" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="E14" s="7" t="n">
+      <c r="E14" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="6" t="n">
         <v>500</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="E15" s="7" t="n">
+      <c r="E15" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="6" t="n">
         <v>500</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="E16" s="7" t="n">
+      <c r="E16" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="6" t="n">
         <v>250</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="E17" s="7" t="n">
+      <c r="E17" s="6" t="n">
         <v>1400</v>
       </c>
-      <c r="F17" s="7" t="n">
+      <c r="F17" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="6" t="n">
         <v>750</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="6" t="n">
         <v>1400</v>
       </c>
-      <c r="E18" s="7" t="n">
+      <c r="E18" s="6" t="n">
         <v>1400</v>
       </c>
-      <c r="F18" s="7" t="n">
+      <c r="F18" s="6" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="6:6">
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="6:6">
-      <c r="F20" s="8"/>
+    <row r="19" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="7"/>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.567568" defaultRowHeight="13.45"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="57.423423" customWidth="1" style="10"/>
-    <col min="3" max="3" width="16.288288" customWidth="1" style="10"/>
-    <col min="4" max="4" width="21.144144" customWidth="1" style="10"/>
-    <col min="5" max="5" width="27.423423" customWidth="1" style="10"/>
-    <col min="6" max="6" width="28.423423" customWidth="1" style="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="5"/>
@@ -2823,20 +2506,20 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="6" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="5"/>
@@ -2846,20 +2529,20 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="6" t="n">
         <v>45</v>
       </c>
       <c r="G3" s="5"/>
@@ -2869,20 +2552,20 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="6" t="n">
         <v>60</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="6" t="n">
         <v>150</v>
       </c>
       <c r="G4" s="5"/>
@@ -2892,20 +2575,20 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>80</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>150</v>
       </c>
       <c r="G5" s="5"/>
@@ -2915,20 +2598,20 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="6" t="n">
         <v>100</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>150</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="6" t="n">
         <v>180</v>
       </c>
       <c r="G6" s="5"/>
@@ -2938,20 +2621,20 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>100</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="6" t="n">
         <v>150</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="6" t="n">
         <v>180</v>
       </c>
       <c r="G7" s="5"/>
@@ -2961,20 +2644,20 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>150</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="6" t="n">
         <v>240</v>
       </c>
       <c r="F8" s="5"/>
@@ -2985,8 +2668,8 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="n">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -3009,7 +2692,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -3023,7 +2706,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -3037,7 +2720,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -3051,7 +2734,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3065,7 +2748,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3079,7 +2762,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -3093,7 +2776,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -3107,7 +2790,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -3121,7 +2804,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -3135,7 +2818,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -3149,7 +2832,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -3163,7 +2846,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3177,7 +2860,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -3191,7 +2874,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3205,7 +2888,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -3219,7 +2902,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -3233,7 +2916,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -3247,7 +2930,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -3261,7 +2944,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3275,7 +2958,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3289,7 +2972,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -3303,7 +2986,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -3317,7 +3000,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -3331,7 +3014,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -3345,7 +3028,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -3359,7 +3042,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -3373,7 +3056,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -3387,7 +3070,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -3401,7 +3084,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3415,7 +3098,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -3429,7 +3112,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3443,7 +3126,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -3457,7 +3140,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -3471,7 +3154,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -3486,32 +3169,12 @@
       <c r="L43" s="5"/>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1722022763" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.787500" right="0.787500" top="1.052778" bottom="1.052778" header="0.787500" footer="0.787500"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman"&amp;12Page &amp;P</oddFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1722022763" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1722022763" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>